<commit_message>
Ajout de la gestion des produits et mise à jour des dépendances
- Ajout d'une structure pour gérer différents types de produits (Fruit, Légume) en utilisant des classes et des dataclasses.
- Implémentation d'un système de factory method pour créer des instances de produits à partir de données structurées.
- Mise à jour du fichier main.py pour inclure un espace pour la fonction principale (à implémenter).
- Ajout de pandas en tant que dépendance pour gérer les données de produits provenant d'un fichier Excel.
- Mise à jour du fichier products.xlsx pour refléter les changements dans la gestion des données de produits.

Ces modifications permettent une meilleure organisation du code et préparent le terrain pour l'ajout de fonctionnalités supplémentaires liées à la gestion des produits.
</commit_message>
<xml_diff>
--- a/src/products.xlsx
+++ b/src/products.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://facylitiesmultiservices-my.sharepoint.com/personal/johnny_neira_fms-ea_com/Documents/Documents/Python/AGM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://facylitiesmultiservices-my.sharepoint.com/personal/johnny_neira_fms-ea_com/Documents/Documents/Python/AGM/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{BFD3BFDC-7638-4B4C-8332-C2DC16ED2A82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60505C29-E2EB-46FA-9A1C-DEC2BE8A14B9}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{BFD3BFDC-7638-4B4C-8332-C2DC16ED2A82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D255DF3-56E3-4172-8CDE-D68DA6243A3B}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-3900" windowWidth="29040" windowHeight="16440" xr2:uid="{0D3599F1-FB10-4553-8A94-B5F1F8E2B7DE}"/>
   </bookViews>
@@ -101,15 +101,9 @@
     <t>Type</t>
   </si>
   <si>
-    <t>Produit</t>
-  </si>
-  <si>
     <t>Fruit</t>
   </si>
   <si>
-    <t>Légumes</t>
-  </si>
-  <si>
     <t>Stock</t>
   </si>
   <si>
@@ -123,14 +117,28 @@
   </si>
   <si>
     <t>Prix /u</t>
+  </si>
+  <si>
+    <t>Nom</t>
+  </si>
+  <si>
+    <t>Légume</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -158,8 +166,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -175,6 +185,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -494,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F059E961-83C1-430E-9663-3B7A5B117B97}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,357 +526,360 @@
         <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2">
+        <v>24</v>
+      </c>
+      <c r="E2" s="2">
         <v>1.3</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3">
+        <v>25</v>
+      </c>
+      <c r="E3" s="2">
         <v>2.5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4">
+        <v>24</v>
+      </c>
+      <c r="E4" s="2">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5">
+        <v>24</v>
+      </c>
+      <c r="E5" s="2">
         <v>2.9</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6">
+        <v>25</v>
+      </c>
+      <c r="E6" s="2">
         <v>2.5</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7">
+        <v>24</v>
+      </c>
+      <c r="E7" s="2">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8">
+        <v>24</v>
+      </c>
+      <c r="E8" s="2">
         <v>2.5</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9">
+        <v>24</v>
+      </c>
+      <c r="E9" s="2">
         <v>2.6</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
         <v>4</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10">
+        <v>24</v>
+      </c>
+      <c r="E10" s="2">
         <v>3.5</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11">
+        <v>24</v>
+      </c>
+      <c r="E11" s="2">
         <v>4.5</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="2">
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12">
+        <v>24</v>
+      </c>
+      <c r="E12" s="2">
         <v>3.5</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="2">
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13">
+        <v>24</v>
+      </c>
+      <c r="E13" s="2">
         <v>2.8</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
         <v>12</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="2">
         <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14">
+        <v>24</v>
+      </c>
+      <c r="E14" s="2">
         <v>1.5</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="2">
         <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15">
+        <v>25</v>
+      </c>
+      <c r="E15" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
         <v>16</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="2">
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16">
+        <v>24</v>
+      </c>
+      <c r="E16" s="2">
         <v>2.5</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B17" t="s">
         <v>13</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="2">
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17">
+        <v>24</v>
+      </c>
+      <c r="E17" s="2">
         <v>1.2</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" t="s">
         <v>18</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="2">
         <v>8</v>
       </c>
       <c r="D18" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18">
+        <v>24</v>
+      </c>
+      <c r="E18" s="2">
         <v>1.5</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
         <v>15</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="2">
         <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>27</v>
-      </c>
-      <c r="E19">
+        <v>25</v>
+      </c>
+      <c r="E19" s="2">
         <v>2.5</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
         <v>17</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="2">
         <v>10</v>
       </c>
       <c r="D20" t="s">
-        <v>27</v>
-      </c>
-      <c r="E20">
+        <v>25</v>
+      </c>
+      <c r="E20" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
         <v>19</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="2">
         <v>3</v>
       </c>
       <c r="D21" t="s">
-        <v>26</v>
-      </c>
-      <c r="E21">
+        <v>24</v>
+      </c>
+      <c r="E21" s="2">
         <v>2.5</v>
       </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E22" s="1"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E21">

</xml_diff>